<commit_message>
pagination for repayment and disbursement
</commit_message>
<xml_diff>
--- a/public/reports_retailer/retailer_comprehensive_reports.xlsx
+++ b/public/reports_retailer/retailer_comprehensive_reports.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Sr.</t>
   </si>
@@ -151,7 +151,7 @@
     <t>Other Local Individuals not mentioned above</t>
   </si>
   <si>
-    <t>Wed Jun 15 2022 15:46:20 GMT+0600 (Bangladesh Standard Time)</t>
+    <t>Sun May 15 2022 15:46:20 GMT+0600 (Bangladesh Standard Time)</t>
   </si>
   <si>
     <t>DHK-99-92</t>
@@ -218,57 +218,6 @@
   </si>
   <si>
     <t>Home / Holding: , Village / Road: TB Clinicpara,, Post Office: Magura-7600, Magura Sadar, Magura</t>
-  </si>
-  <si>
-    <t>DHK-99-98</t>
-  </si>
-  <si>
-    <t>0100000000006989</t>
-  </si>
-  <si>
-    <t>MD. RASEL MIA</t>
-  </si>
-  <si>
-    <t>Md. AH Hai</t>
-  </si>
-  <si>
-    <t>Mrs. Rabia Begum</t>
-  </si>
-  <si>
-    <t>Mon Mar 15 1993 06:00:00 GMT+0600 (Bangladesh Standard Time)</t>
-  </si>
-  <si>
-    <t>Sherpur</t>
-  </si>
-  <si>
-    <t>Home / Holding: Dikpara, Village / Road: , Char birding, Post Office: Dikpara-2100, Sherpur Sadar, Sherpur</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0100000000007290</t>
-  </si>
-  <si>
-    <t>Coca Distributor</t>
-  </si>
-  <si>
-    <t>Wed Jun 15 2022 15:46:21 GMT+0600 (Bangladesh Standard Time)</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0100000000008590</t>
-  </si>
-  <si>
-    <t>DHK-1</t>
-  </si>
-  <si>
-    <t>0100000000002260</t>
-  </si>
-  <si>
-    <t>Wed Jun 15 2022 16:22:42 GMT+0600 (Bangladesh Standard Time)</t>
   </si>
 </sst>
 </file>
@@ -330,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG25"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -543,10 +492,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>35</v>
@@ -558,19 +507,19 @@
         <v>35</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>35</v>
@@ -582,28 +531,28 @@
         <v>39</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>1234567891</v>
+        <v>2695047100000</v>
       </c>
       <c r="S3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="W3" s="0" t="s">
         <v>42</v>
@@ -644,10 +593,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>35</v>
@@ -659,19 +608,19 @@
         <v>35</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>35</v>
@@ -683,28 +632,28 @@
         <v>39</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Q4" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>1234567892</v>
+        <v>2695047100000</v>
       </c>
       <c r="S4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="W4" s="0" t="s">
         <v>42</v>
@@ -745,10 +694,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>35</v>
@@ -760,19 +709,19 @@
         <v>35</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>35</v>
@@ -784,28 +733,28 @@
         <v>39</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Q5" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>1234567893</v>
+        <v>2695047100000</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="U5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="W5" s="0" t="s">
         <v>42</v>
@@ -846,10 +795,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>35</v>
@@ -861,19 +810,19 @@
         <v>35</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>35</v>
@@ -885,28 +834,28 @@
         <v>39</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="Q6" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>1234567894</v>
+        <v>1234567891</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="U6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="W6" s="0" t="s">
         <v>42</v>
@@ -947,10 +896,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>35</v>
@@ -962,19 +911,19 @@
         <v>35</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>35</v>
@@ -986,28 +935,28 @@
         <v>39</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>2695047100000</v>
+        <v>1234567891</v>
       </c>
       <c r="S7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="U7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="W7" s="0" t="s">
         <v>42</v>
@@ -1149,10 +1098,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>35</v>
@@ -1164,19 +1113,19 @@
         <v>35</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>35</v>
@@ -1188,7 +1137,7 @@
         <v>39</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="P9" s="0" t="s">
         <v>53</v>
@@ -1197,13 +1146,13 @@
         <v>42</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>1234567892</v>
+        <v>1234567891</v>
       </c>
       <c r="S9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="U9" s="0" t="n">
         <v>0</v>
@@ -1250,10 +1199,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>35</v>
@@ -1265,19 +1214,19 @@
         <v>35</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>35</v>
@@ -1289,7 +1238,7 @@
         <v>39</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="P10" s="0" t="s">
         <v>53</v>
@@ -1298,13 +1247,13 @@
         <v>42</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>1234567893</v>
+        <v>1234567892</v>
       </c>
       <c r="S10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="U10" s="0" t="n">
         <v>0</v>
@@ -1351,10 +1300,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>35</v>
@@ -1366,19 +1315,19 @@
         <v>35</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>35</v>
@@ -1390,28 +1339,28 @@
         <v>39</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>1234567894</v>
+        <v>1234567892</v>
       </c>
       <c r="S11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="U11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="W11" s="0" t="s">
         <v>42</v>
@@ -1452,10 +1401,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>35</v>
@@ -1467,19 +1416,19 @@
         <v>35</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>35</v>
@@ -1491,28 +1440,28 @@
         <v>39</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>2695047100000</v>
+        <v>1234567892</v>
       </c>
       <c r="S12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V12" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="W12" s="0" t="s">
         <v>42</v>
@@ -1553,10 +1502,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>35</v>
@@ -1568,19 +1517,19 @@
         <v>35</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>35</v>
@@ -1592,7 +1541,7 @@
         <v>39</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="P13" s="0" t="s">
         <v>53</v>
@@ -1601,13 +1550,13 @@
         <v>42</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>1234567891</v>
+        <v>1234567892</v>
       </c>
       <c r="S13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>0</v>
@@ -1654,10 +1603,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>35</v>
@@ -1669,19 +1618,19 @@
         <v>35</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>35</v>
@@ -1693,7 +1642,7 @@
         <v>39</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="P14" s="0" t="s">
         <v>53</v>
@@ -1702,13 +1651,13 @@
         <v>42</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>1234567892</v>
+        <v>1234567893</v>
       </c>
       <c r="S14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>0</v>
@@ -1856,10 +1805,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>35</v>
@@ -1871,19 +1820,19 @@
         <v>35</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>35</v>
@@ -1895,28 +1844,28 @@
         <v>39</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="Q16" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R16" s="0" t="n">
-        <v>1234567894</v>
+        <v>1234567893</v>
       </c>
       <c r="S16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T16" s="0" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="U16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V16" s="0" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="W16" s="0" t="s">
         <v>42</v>
@@ -1957,10 +1906,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>35</v>
@@ -1972,19 +1921,19 @@
         <v>35</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>35</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>35</v>
@@ -1996,28 +1945,28 @@
         <v>39</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="Q17" s="0" t="s">
         <v>42</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>2695047100000</v>
+        <v>1234567893</v>
       </c>
       <c r="S17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="U17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="W17" s="0" t="s">
         <v>42</v>
@@ -2050,814 +1999,6 @@
         <v>46</v>
       </c>
       <c r="AG17" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:33">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R18" s="0" t="n">
-        <v>1234567891</v>
-      </c>
-      <c r="S18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="W18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC18" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG18" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33">
-      <c r="A19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="P19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R19" s="0" t="n">
-        <v>1234567892</v>
-      </c>
-      <c r="S19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="U19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="W19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC19" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD19" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF19" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG19" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:33">
-      <c r="A20" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q20" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R20" s="0" t="n">
-        <v>1234567893</v>
-      </c>
-      <c r="S20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="U20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="W20" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA20" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC20" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD20" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF20" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG20" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:33">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="P21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q21" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R21" s="0" t="n">
-        <v>1234567894</v>
-      </c>
-      <c r="S21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="U21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="W21" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA21" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC21" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD21" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF21" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG21" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:33">
-      <c r="A22" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="P22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R22" s="0" t="n">
-        <v>8765098764</v>
-      </c>
-      <c r="S22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="U22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="W22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC22" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD22" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF22" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG22" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:33">
-      <c r="A23" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="P23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R23" s="0" t="n">
-        <v>4673209876</v>
-      </c>
-      <c r="S23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="W23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC23" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF23" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG23" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:33">
-      <c r="A24" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="P24" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="R24" s="0" t="n">
-        <v>4673209876</v>
-      </c>
-      <c r="S24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T24" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="W24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="X24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC24" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF24" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG24" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33">
-      <c r="A25" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="O25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="R25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="W25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="X25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC25" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF25" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG25" s="0" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>